<commit_message>
Address code and configs updated
</commit_message>
<xml_diff>
--- a/Config/Singapore_Financial_Config.xlsx
+++ b/Config/Singapore_Financial_Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRADSOL123\PycharmProjects\MNS-Singapore\MNS-Singapore\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16705375-3B40-4842-91CC-936F2EDA3F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE6F092-264E-47FB-BB45-B37CCADEE6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1245" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$315</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$319</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2232" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2256" uniqueCount="608">
   <si>
     <t>Field_Name</t>
   </si>
@@ -1596,9 +1596,6 @@
     <t>Marketing and distribution expenses</t>
   </si>
   <si>
-    <t>selling_expenses+selling_expense+selling_and_distribution_expenses+distribution_expenses+distribution_costs+selling_and_marketing_expenses+distribution_and_marketing+marketing_and_distribution_expenses</t>
-  </si>
-  <si>
     <t>administrative_expenses</t>
   </si>
   <si>
@@ -1704,9 +1701,6 @@
     <t>Income tax credit/(expense)</t>
   </si>
   <si>
-    <t>income_tax_expense+income_tax_expenses+income_tax+tax_benefit_expense+income_tax_benefit_expense+tax_expense+taxation+income_tax_credit_expense</t>
-  </si>
-  <si>
     <t>minority_interest_and_profit_from_associates_and_joint_ventures</t>
   </si>
   <si>
@@ -1767,9 +1761,6 @@
     <t>Other_income</t>
   </si>
   <si>
-    <t>Other_income+other_income_gains_and_losses+other_gains_net+other_income_and_gains+Other_income_net</t>
-  </si>
-  <si>
     <t>financial_assets_at_fvoci</t>
   </si>
   <si>
@@ -1822,6 +1813,45 @@
   </si>
   <si>
     <t>current_tax_liabilities+current_tax_payable+tax_liabilities+current_income_tax_liabilities+provision_for_taxation+income_tax_payables+Tax_payable</t>
+  </si>
+  <si>
+    <t>Share of results of equity-accounted investees, net of tax</t>
+  </si>
+  <si>
+    <t>Share_of_results_of_equity_accounted_investees_net_of_tax</t>
+  </si>
+  <si>
+    <t>Other_income+other_income_gains_and_losses+other_gains_net+other_income_and_gains+Other_income_net+Share_of_results_of_equity_accounted_investees_net_of_tax</t>
+  </si>
+  <si>
+    <t>financial_income</t>
+  </si>
+  <si>
+    <t>Interest income</t>
+  </si>
+  <si>
+    <t>Interest_income</t>
+  </si>
+  <si>
+    <t>Finance income+Interest_income</t>
+  </si>
+  <si>
+    <t>Selling_expenses</t>
+  </si>
+  <si>
+    <t>Selling, distribution and outlet expenses</t>
+  </si>
+  <si>
+    <t>Selling_distribution_and_outlet_expenses</t>
+  </si>
+  <si>
+    <t>Selling_expenses+selling_expense+selling_and_distribution_expenses+distribution_expenses+distribution_costs+selling_and_marketing_expenses+distribution_and_marketing+marketing_and_distribution_expenses+Selling_distribution_and_outlet_expenses</t>
+  </si>
+  <si>
+    <t>Income_tax</t>
+  </si>
+  <si>
+    <t>income_tax_expense+income_tax_expenses+Income_tax+tax_benefit_expense+income_tax_benefit_expense+tax_expense+taxation+income_tax_credit_expense</t>
   </si>
 </sst>
 </file>
@@ -1944,7 +1974,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1979,6 +2009,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2261,10 +2297,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H347"/>
+  <dimension ref="A1:H351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
-      <selection activeCell="C266" sqref="C266"/>
+    <sheetView tabSelected="1" topLeftCell="A336" workbookViewId="0">
+      <selection activeCell="B342" sqref="B342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2640,7 +2676,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>135</v>
@@ -2715,7 +2751,7 @@
         <v>136</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D23" t="s">
         <v>134</v>
@@ -2801,13 +2837,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="D27" t="s">
         <v>134</v>
@@ -2824,13 +2860,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="D28" t="s">
         <v>134</v>
@@ -2853,7 +2889,7 @@
         <v>136</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D29" t="s">
         <v>134</v>
@@ -3491,13 +3527,13 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D57" t="s">
         <v>134</v>
@@ -3514,13 +3550,13 @@
     </row>
     <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="D58" t="s">
         <v>134</v>
@@ -3543,7 +3579,7 @@
         <v>136</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D59" t="s">
         <v>134</v>
@@ -3767,13 +3803,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D69" t="s">
         <v>134</v>
@@ -3796,7 +3832,7 @@
         <v>136</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D70" t="s">
         <v>134</v>
@@ -4296,13 +4332,13 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D92" t="s">
         <v>134</v>
@@ -4325,7 +4361,7 @@
         <v>136</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D93" t="s">
         <v>134</v>
@@ -5055,13 +5091,13 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D125" t="s">
         <v>134</v>
@@ -5084,7 +5120,7 @@
         <v>136</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D126" t="s">
         <v>134</v>
@@ -5226,13 +5262,13 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="D134" t="s">
         <v>134</v>
@@ -5249,13 +5285,13 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D135" t="s">
         <v>134</v>
@@ -5278,7 +5314,7 @@
         <v>136</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="D136" t="s">
         <v>134</v>
@@ -5548,13 +5584,13 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B148" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D148" t="s">
         <v>134</v>
@@ -5577,7 +5613,7 @@
         <v>136</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D149" t="s">
         <v>134</v>
@@ -5847,13 +5883,13 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B161" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D161" t="s">
         <v>134</v>
@@ -5876,7 +5912,7 @@
         <v>136</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D162" t="s">
         <v>134</v>
@@ -6054,13 +6090,13 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B170" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C170" s="6" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D170" t="s">
         <v>134</v>
@@ -6083,7 +6119,7 @@
         <v>136</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D171" t="s">
         <v>134</v>
@@ -6560,13 +6596,13 @@
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="6" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B192" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C192" s="6" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D192" t="s">
         <v>134</v>
@@ -6589,7 +6625,7 @@
         <v>136</v>
       </c>
       <c r="C193" s="6" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D193" t="s">
         <v>134</v>
@@ -6836,13 +6872,13 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="6" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B204" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C204" s="6" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="D204" t="s">
         <v>134</v>
@@ -6865,7 +6901,7 @@
         <v>136</v>
       </c>
       <c r="C205" s="6" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="D205" t="s">
         <v>134</v>
@@ -7181,13 +7217,13 @@
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B219" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C219" s="6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D219" t="s">
         <v>134</v>
@@ -7210,7 +7246,7 @@
         <v>136</v>
       </c>
       <c r="C220" s="6" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D220" t="s">
         <v>134</v>
@@ -8087,7 +8123,7 @@
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267" s="6" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B267" s="6" t="s">
         <v>135</v>
@@ -8167,13 +8203,13 @@
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271" s="6" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B271" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C271" s="6" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D271" t="s">
         <v>134</v>
@@ -8187,33 +8223,33 @@
     </row>
     <row r="272" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B272" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C272" s="6" t="s">
+        <v>595</v>
+      </c>
+      <c r="D272" t="s">
+        <v>134</v>
+      </c>
+      <c r="E272" t="s">
+        <v>147</v>
+      </c>
+      <c r="H272" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A273" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B272" s="6" t="s">
+      <c r="B273" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C272" s="6" t="s">
-        <v>579</v>
-      </c>
-      <c r="D272" t="s">
-        <v>134</v>
-      </c>
-      <c r="E272" t="s">
-        <v>147</v>
-      </c>
-      <c r="H272" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A273" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B273" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C273" s="13" t="s">
-        <v>29</v>
+      <c r="C273" s="6" t="s">
+        <v>597</v>
       </c>
       <c r="D273" t="s">
         <v>134</v>
@@ -8227,13 +8263,13 @@
     </row>
     <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B274" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C274" s="13" t="s">
-        <v>497</v>
+        <v>29</v>
       </c>
       <c r="D274" t="s">
         <v>134</v>
@@ -8247,93 +8283,93 @@
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B275" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C275" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="D275" t="s">
+        <v>134</v>
+      </c>
+      <c r="E275" t="s">
+        <v>147</v>
+      </c>
+      <c r="H275" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A276" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B275" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C275" s="13" t="s">
+      <c r="B276" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C276" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D275" t="s">
-        <v>134</v>
-      </c>
-      <c r="E275" t="s">
-        <v>147</v>
-      </c>
-      <c r="H275" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A276" s="6" t="s">
+      <c r="D276" t="s">
+        <v>134</v>
+      </c>
+      <c r="E276" t="s">
+        <v>147</v>
+      </c>
+      <c r="H276" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A277" s="14" t="s">
+        <v>598</v>
+      </c>
+      <c r="B277" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C277" s="15" t="s">
+        <v>498</v>
+      </c>
+      <c r="D277" t="s">
+        <v>134</v>
+      </c>
+      <c r="E277" t="s">
+        <v>147</v>
+      </c>
+      <c r="H277" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A278" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="B278" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C278" s="15" t="s">
+        <v>599</v>
+      </c>
+      <c r="D278" t="s">
+        <v>134</v>
+      </c>
+      <c r="E278" t="s">
+        <v>147</v>
+      </c>
+      <c r="H278" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A279" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="B276" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C276" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="D276" t="s">
-        <v>134</v>
-      </c>
-      <c r="E276" t="s">
-        <v>147</v>
-      </c>
-      <c r="H276" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="277" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A277" s="6" t="s">
-        <v>499</v>
-      </c>
-      <c r="B277" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C277" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="D277" t="s">
-        <v>134</v>
-      </c>
-      <c r="E277" t="s">
-        <v>147</v>
-      </c>
-      <c r="H277" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="278" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A278" s="6" t="s">
-        <v>501</v>
-      </c>
-      <c r="B278" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C278" s="6" t="s">
-        <v>502</v>
-      </c>
-      <c r="D278" t="s">
-        <v>134</v>
-      </c>
-      <c r="E278" t="s">
-        <v>147</v>
-      </c>
-      <c r="H278" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="279" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A279" s="6" t="s">
-        <v>100</v>
       </c>
       <c r="B279" s="6" t="s">
         <v>136</v>
       </c>
       <c r="C279" s="6" t="s">
-        <v>503</v>
+        <v>601</v>
       </c>
       <c r="D279" t="s">
         <v>134</v>
@@ -8347,13 +8383,13 @@
     </row>
     <row r="280" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A280" s="6" t="s">
-        <v>101</v>
+        <v>499</v>
       </c>
       <c r="B280" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C280" s="6" t="s">
-        <v>29</v>
+        <v>500</v>
       </c>
       <c r="D280" t="s">
         <v>134</v>
@@ -8365,15 +8401,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A281" s="6" t="s">
-        <v>102</v>
+        <v>501</v>
       </c>
       <c r="B281" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C281" s="6" t="s">
-        <v>29</v>
+        <v>502</v>
       </c>
       <c r="D281" t="s">
         <v>134</v>
@@ -8387,13 +8423,13 @@
     </row>
     <row r="282" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A282" s="6" t="s">
-        <v>504</v>
+        <v>100</v>
       </c>
       <c r="B282" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C282" s="6" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D282" t="s">
         <v>134</v>
@@ -8407,93 +8443,93 @@
     </row>
     <row r="283" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A283" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B283" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C283" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D283" t="s">
+        <v>134</v>
+      </c>
+      <c r="E283" t="s">
+        <v>147</v>
+      </c>
+      <c r="H283" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A284" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B284" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C284" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D284" t="s">
+        <v>134</v>
+      </c>
+      <c r="E284" t="s">
+        <v>147</v>
+      </c>
+      <c r="H284" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A285" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="B285" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C285" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="D285" t="s">
+        <v>134</v>
+      </c>
+      <c r="E285" t="s">
+        <v>147</v>
+      </c>
+      <c r="H285" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A286" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="B283" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C283" s="6" t="s">
+      <c r="B286" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C286" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="D283" t="s">
-        <v>134</v>
-      </c>
-      <c r="E283" t="s">
-        <v>147</v>
-      </c>
-      <c r="H283" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="284" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A284" s="6" t="s">
+      <c r="D286" t="s">
+        <v>134</v>
+      </c>
+      <c r="E286" t="s">
+        <v>147</v>
+      </c>
+      <c r="H286" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A287" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B284" s="6" t="s">
+      <c r="B287" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C284" s="6" t="s">
+      <c r="C287" s="6" t="s">
         <v>508</v>
-      </c>
-      <c r="D284" t="s">
-        <v>134</v>
-      </c>
-      <c r="E284" t="s">
-        <v>147</v>
-      </c>
-      <c r="H284" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A285" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B285" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C285" s="6" t="s">
-        <v>509</v>
-      </c>
-      <c r="D285" t="s">
-        <v>134</v>
-      </c>
-      <c r="E285" t="s">
-        <v>147</v>
-      </c>
-      <c r="H285" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A286" s="6" t="s">
-        <v>510</v>
-      </c>
-      <c r="B286" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C286" s="6" t="s">
-        <v>511</v>
-      </c>
-      <c r="D286" t="s">
-        <v>134</v>
-      </c>
-      <c r="E286" t="s">
-        <v>147</v>
-      </c>
-      <c r="H286" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="287" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A287" s="6" t="s">
-        <v>512</v>
-      </c>
-      <c r="B287" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C287" s="6" t="s">
-        <v>513</v>
       </c>
       <c r="D287" t="s">
         <v>134</v>
@@ -8507,13 +8543,13 @@
     </row>
     <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288" s="6" t="s">
-        <v>270</v>
+        <v>602</v>
       </c>
       <c r="B288" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C288" s="6" t="s">
-        <v>271</v>
+        <v>509</v>
       </c>
       <c r="D288" t="s">
         <v>134</v>
@@ -8527,13 +8563,13 @@
     </row>
     <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289" s="6" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="B289" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C289" s="6" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D289" t="s">
         <v>134</v>
@@ -8545,15 +8581,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A290" s="6" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="B290" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C290" s="6" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="D290" t="s">
         <v>134</v>
@@ -8567,13 +8603,13 @@
     </row>
     <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291" s="6" t="s">
-        <v>518</v>
+        <v>270</v>
       </c>
       <c r="B291" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C291" s="6" t="s">
-        <v>519</v>
+        <v>271</v>
       </c>
       <c r="D291" t="s">
         <v>134</v>
@@ -8585,15 +8621,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="292" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292" s="6" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="B292" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C292" s="6" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="D292" t="s">
         <v>134</v>
@@ -8605,15 +8641,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="293" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293" s="6" t="s">
-        <v>104</v>
+        <v>516</v>
       </c>
       <c r="B293" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C293" s="6" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="D293" t="s">
         <v>134</v>
@@ -8627,93 +8663,93 @@
     </row>
     <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="B294" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C294" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="D294" t="s">
+        <v>134</v>
+      </c>
+      <c r="E294" t="s">
+        <v>147</v>
+      </c>
+      <c r="H294" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="295" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A295" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="B295" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C295" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="D295" t="s">
+        <v>134</v>
+      </c>
+      <c r="E295" t="s">
+        <v>147</v>
+      </c>
+      <c r="H295" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A296" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="B296" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C296" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="D296" t="s">
+        <v>134</v>
+      </c>
+      <c r="E296" t="s">
+        <v>147</v>
+      </c>
+      <c r="H296" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="297" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A297" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B297" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C297" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="D297" t="s">
+        <v>134</v>
+      </c>
+      <c r="E297" t="s">
+        <v>147</v>
+      </c>
+      <c r="H297" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A298" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="B298" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C298" s="6" t="s">
         <v>523</v>
-      </c>
-      <c r="B294" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C294" s="6" t="s">
-        <v>524</v>
-      </c>
-      <c r="D294" t="s">
-        <v>134</v>
-      </c>
-      <c r="E294" t="s">
-        <v>147</v>
-      </c>
-      <c r="H294" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A295" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="B295" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C295" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="D295" t="s">
-        <v>134</v>
-      </c>
-      <c r="E295" t="s">
-        <v>147</v>
-      </c>
-      <c r="H295" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A296" s="6" t="s">
-        <v>525</v>
-      </c>
-      <c r="B296" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C296" s="6" t="s">
-        <v>526</v>
-      </c>
-      <c r="D296" t="s">
-        <v>134</v>
-      </c>
-      <c r="E296" t="s">
-        <v>147</v>
-      </c>
-      <c r="H296" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="297" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A297" s="6" t="s">
-        <v>527</v>
-      </c>
-      <c r="B297" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C297" s="6" t="s">
-        <v>528</v>
-      </c>
-      <c r="D297" t="s">
-        <v>134</v>
-      </c>
-      <c r="E297" t="s">
-        <v>147</v>
-      </c>
-      <c r="H297" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="298" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A298" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B298" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C298" s="6" t="s">
-        <v>529</v>
       </c>
       <c r="D298" t="s">
         <v>134</v>
@@ -8727,13 +8763,13 @@
     </row>
     <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B299" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C299" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D299" t="s">
         <v>134</v>
@@ -8747,13 +8783,13 @@
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300" s="6" t="s">
-        <v>276</v>
+        <v>524</v>
       </c>
       <c r="B300" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C300" s="6" t="s">
-        <v>277</v>
+        <v>525</v>
       </c>
       <c r="D300" t="s">
         <v>134</v>
@@ -8765,35 +8801,35 @@
         <v>150</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A301" s="6" t="s">
-        <v>106</v>
+        <v>526</v>
       </c>
       <c r="B301" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C301" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="D301" t="s">
+        <v>134</v>
+      </c>
+      <c r="E301" t="s">
+        <v>147</v>
+      </c>
+      <c r="H301" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A302" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B302" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C301" s="6" t="s">
-        <v>530</v>
-      </c>
-      <c r="D301" t="s">
-        <v>134</v>
-      </c>
-      <c r="E301" t="s">
-        <v>147</v>
-      </c>
-      <c r="H301" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A302" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B302" s="6" t="s">
-        <v>135</v>
-      </c>
       <c r="C302" s="6" t="s">
-        <v>29</v>
+        <v>528</v>
       </c>
       <c r="D302" t="s">
         <v>134</v>
@@ -8807,13 +8843,13 @@
     </row>
     <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A303" s="6" t="s">
-        <v>108</v>
+        <v>274</v>
       </c>
       <c r="B303" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C303" s="6" t="s">
-        <v>29</v>
+        <v>275</v>
       </c>
       <c r="D303" t="s">
         <v>134</v>
@@ -8827,13 +8863,13 @@
     </row>
     <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304" s="6" t="s">
-        <v>109</v>
+        <v>276</v>
       </c>
       <c r="B304" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C304" s="6" t="s">
-        <v>29</v>
+        <v>277</v>
       </c>
       <c r="D304" t="s">
         <v>134</v>
@@ -8847,13 +8883,13 @@
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B305" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C305" s="6" t="s">
-        <v>29</v>
+        <v>529</v>
       </c>
       <c r="D305" t="s">
         <v>134</v>
@@ -8867,7 +8903,7 @@
     </row>
     <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B306" s="6" t="s">
         <v>135</v>
@@ -8887,7 +8923,7 @@
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307" s="6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B307" s="6" t="s">
         <v>135</v>
@@ -8905,15 +8941,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="308" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308" s="6" t="s">
-        <v>278</v>
+        <v>109</v>
       </c>
       <c r="B308" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C308" s="6" t="s">
-        <v>279</v>
+        <v>29</v>
       </c>
       <c r="D308" t="s">
         <v>134</v>
@@ -8927,133 +8963,133 @@
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B309" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C309" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D309" t="s">
+        <v>134</v>
+      </c>
+      <c r="E309" t="s">
+        <v>147</v>
+      </c>
+      <c r="H309" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A310" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B310" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C310" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D310" t="s">
+        <v>134</v>
+      </c>
+      <c r="E310" t="s">
+        <v>147</v>
+      </c>
+      <c r="H310" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A311" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B311" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C311" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D311" t="s">
+        <v>134</v>
+      </c>
+      <c r="E311" t="s">
+        <v>147</v>
+      </c>
+      <c r="H311" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="312" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A312" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="B312" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C312" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D312" t="s">
+        <v>134</v>
+      </c>
+      <c r="E312" t="s">
+        <v>147</v>
+      </c>
+      <c r="H312" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A313" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="B313" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C313" s="6" t="s">
         <v>531</v>
       </c>
-      <c r="B309" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C309" s="6" t="s">
+      <c r="D313" t="s">
+        <v>134</v>
+      </c>
+      <c r="E313" t="s">
+        <v>147</v>
+      </c>
+      <c r="H313" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="314" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A314" s="6" t="s">
         <v>532</v>
       </c>
-      <c r="D309" t="s">
-        <v>134</v>
-      </c>
-      <c r="E309" t="s">
-        <v>147</v>
-      </c>
-      <c r="H309" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="310" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A310" s="6" t="s">
+      <c r="B314" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C314" s="6" t="s">
         <v>533</v>
       </c>
-      <c r="B310" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C310" s="6" t="s">
+      <c r="D314" t="s">
+        <v>134</v>
+      </c>
+      <c r="E314" t="s">
+        <v>147</v>
+      </c>
+      <c r="H314" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="315" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A315" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="D310" t="s">
-        <v>134</v>
-      </c>
-      <c r="E310" t="s">
-        <v>147</v>
-      </c>
-      <c r="H310" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="311" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A311" s="6" t="s">
+      <c r="B315" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C315" s="6" t="s">
         <v>535</v>
-      </c>
-      <c r="B311" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C311" s="6" t="s">
-        <v>536</v>
-      </c>
-      <c r="D311" t="s">
-        <v>134</v>
-      </c>
-      <c r="E311" t="s">
-        <v>147</v>
-      </c>
-      <c r="H311" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A312" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B312" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C312" s="6" t="s">
-        <v>537</v>
-      </c>
-      <c r="D312" t="s">
-        <v>134</v>
-      </c>
-      <c r="E312" t="s">
-        <v>147</v>
-      </c>
-      <c r="H312" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="313" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A313" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="B313" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C313" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="D313" t="s">
-        <v>134</v>
-      </c>
-      <c r="E313" t="s">
-        <v>147</v>
-      </c>
-      <c r="H313" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="314" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A314" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B314" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C314" s="6" t="s">
-        <v>538</v>
-      </c>
-      <c r="D314" t="s">
-        <v>134</v>
-      </c>
-      <c r="E314" t="s">
-        <v>147</v>
-      </c>
-      <c r="H314" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A315" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B315" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C315" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="D315" t="s">
         <v>134</v>
@@ -9067,73 +9103,73 @@
     </row>
     <row r="316" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A316" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B316" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C316" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="D316" t="s">
+        <v>134</v>
+      </c>
+      <c r="E316" t="s">
+        <v>147</v>
+      </c>
+      <c r="H316" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="317" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A317" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="B317" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C317" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="D317" t="s">
+        <v>134</v>
+      </c>
+      <c r="E317" t="s">
+        <v>147</v>
+      </c>
+      <c r="H317" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="318" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A318" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B318" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C318" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="D318" t="s">
+        <v>134</v>
+      </c>
+      <c r="E318" t="s">
+        <v>147</v>
+      </c>
+      <c r="H318" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A319" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B319" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C319" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="D316" t="s">
-        <v>134</v>
-      </c>
-      <c r="E316" t="s">
-        <v>147</v>
-      </c>
-      <c r="H316" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A317" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B317" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C317" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D317" t="s">
-        <v>134</v>
-      </c>
-      <c r="E317" t="s">
-        <v>147</v>
-      </c>
-      <c r="H317" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="318" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A318" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B318" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C318" s="6" t="s">
-        <v>539</v>
-      </c>
-      <c r="D318" t="s">
-        <v>134</v>
-      </c>
-      <c r="E318" t="s">
-        <v>147</v>
-      </c>
-      <c r="H318" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="319" spans="1:8" ht="195" x14ac:dyDescent="0.25">
-      <c r="A319" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="B319" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C319" s="6" t="s">
-        <v>282</v>
       </c>
       <c r="D319" t="s">
         <v>134</v>
@@ -9147,13 +9183,13 @@
     </row>
     <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320" s="6" t="s">
-        <v>540</v>
+        <v>115</v>
       </c>
       <c r="B320" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C320" s="6" t="s">
-        <v>541</v>
+        <v>29</v>
       </c>
       <c r="D320" t="s">
         <v>134</v>
@@ -9167,13 +9203,13 @@
     </row>
     <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321" s="6" t="s">
-        <v>284</v>
+        <v>116</v>
       </c>
       <c r="B321" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C321" s="6" t="s">
-        <v>149</v>
+        <v>29</v>
       </c>
       <c r="D321" t="s">
         <v>134</v>
@@ -9185,15 +9221,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A322" s="6" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="B322" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C322" s="6" t="s">
-        <v>283</v>
+        <v>538</v>
       </c>
       <c r="D322" t="s">
         <v>134</v>
@@ -9205,15 +9241,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A323" s="6" t="s">
-        <v>542</v>
+        <v>118</v>
       </c>
       <c r="B323" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C323" s="6" t="s">
-        <v>543</v>
+        <v>282</v>
       </c>
       <c r="D323" t="s">
         <v>134</v>
@@ -9227,13 +9263,13 @@
     </row>
     <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324" s="6" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="B324" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C324" s="6" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="D324" t="s">
         <v>134</v>
@@ -9245,15 +9281,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="325" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A325" s="6" t="s">
-        <v>119</v>
+        <v>284</v>
       </c>
       <c r="B325" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C325" s="6" t="s">
-        <v>546</v>
+        <v>149</v>
       </c>
       <c r="D325" t="s">
         <v>134</v>
@@ -9267,13 +9303,13 @@
     </row>
     <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326" s="6" t="s">
-        <v>120</v>
+        <v>148</v>
       </c>
       <c r="B326" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C326" s="6" t="s">
-        <v>29</v>
+        <v>283</v>
       </c>
       <c r="D326" t="s">
         <v>134</v>
@@ -9285,15 +9321,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="327" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327" s="6" t="s">
-        <v>121</v>
+        <v>541</v>
       </c>
       <c r="B327" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C327" s="6" t="s">
-        <v>122</v>
+        <v>542</v>
       </c>
       <c r="D327" t="s">
         <v>134</v>
@@ -9307,13 +9343,13 @@
     </row>
     <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328" s="6" t="s">
-        <v>123</v>
+        <v>543</v>
       </c>
       <c r="B328" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C328" s="6" t="s">
-        <v>29</v>
+        <v>544</v>
       </c>
       <c r="D328" t="s">
         <v>134</v>
@@ -9327,13 +9363,13 @@
     </row>
     <row r="329" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A329" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B329" s="6" t="s">
         <v>136</v>
       </c>
       <c r="C329" s="6" t="s">
-        <v>285</v>
+        <v>545</v>
       </c>
       <c r="D329" t="s">
         <v>134</v>
@@ -9347,13 +9383,13 @@
     </row>
     <row r="330" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A330" s="6" t="s">
-        <v>286</v>
+        <v>120</v>
       </c>
       <c r="B330" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C330" s="6" t="s">
-        <v>287</v>
+        <v>29</v>
       </c>
       <c r="D330" t="s">
         <v>134</v>
@@ -9365,15 +9401,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A331" s="6" t="s">
-        <v>288</v>
+        <v>121</v>
       </c>
       <c r="B331" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C331" s="6" t="s">
-        <v>289</v>
+        <v>122</v>
       </c>
       <c r="D331" t="s">
         <v>134</v>
@@ -9387,13 +9423,13 @@
     </row>
     <row r="332" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A332" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B332" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C332" s="6" t="s">
-        <v>547</v>
+        <v>29</v>
       </c>
       <c r="D332" t="s">
         <v>134</v>
@@ -9405,15 +9441,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A333" s="6" t="s">
-        <v>548</v>
+        <v>124</v>
       </c>
       <c r="B333" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C333" s="6" t="s">
-        <v>549</v>
+        <v>285</v>
       </c>
       <c r="D333" t="s">
         <v>134</v>
@@ -9427,13 +9463,13 @@
     </row>
     <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334" s="6" t="s">
-        <v>550</v>
+        <v>286</v>
       </c>
       <c r="B334" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C334" s="6" t="s">
-        <v>551</v>
+        <v>287</v>
       </c>
       <c r="D334" t="s">
         <v>134</v>
@@ -9447,13 +9483,13 @@
     </row>
     <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335" s="6" t="s">
-        <v>552</v>
+        <v>288</v>
       </c>
       <c r="B335" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C335" s="6" t="s">
-        <v>553</v>
+        <v>289</v>
       </c>
       <c r="D335" t="s">
         <v>134</v>
@@ -9467,13 +9503,13 @@
     </row>
     <row r="336" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A336" s="6" t="s">
-        <v>554</v>
+        <v>606</v>
       </c>
       <c r="B336" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C336" s="6" t="s">
-        <v>555</v>
+        <v>546</v>
       </c>
       <c r="D336" t="s">
         <v>134</v>
@@ -9487,13 +9523,13 @@
     </row>
     <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337" s="6" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
       <c r="B337" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C337" s="6" t="s">
-        <v>557</v>
+        <v>548</v>
       </c>
       <c r="D337" t="s">
         <v>134</v>
@@ -9505,15 +9541,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="338" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338" s="6" t="s">
-        <v>125</v>
+        <v>549</v>
       </c>
       <c r="B338" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C338" s="6" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
       <c r="D338" t="s">
         <v>134</v>
@@ -9525,15 +9561,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="339" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339" s="6" t="s">
-        <v>130</v>
+        <v>551</v>
       </c>
       <c r="B339" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C339" s="6" t="s">
-        <v>29</v>
+        <v>552</v>
       </c>
       <c r="D339" t="s">
         <v>134</v>
@@ -9545,15 +9581,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="340" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A340" s="6" t="s">
-        <v>131</v>
+        <v>553</v>
       </c>
       <c r="B340" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C340" s="6" t="s">
-        <v>29</v>
+        <v>554</v>
       </c>
       <c r="D340" t="s">
         <v>134</v>
@@ -9567,13 +9603,13 @@
     </row>
     <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341" s="6" t="s">
-        <v>126</v>
+        <v>555</v>
       </c>
       <c r="B341" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C341" s="6" t="s">
-        <v>29</v>
+        <v>556</v>
       </c>
       <c r="D341" t="s">
         <v>134</v>
@@ -9585,15 +9621,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A342" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B342" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C342" s="6" t="s">
-        <v>29</v>
+        <v>607</v>
       </c>
       <c r="D342" t="s">
         <v>134</v>
@@ -9605,9 +9641,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A343" s="6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B343" s="6" t="s">
         <v>135</v>
@@ -9625,9 +9661,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A344" s="6" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B344" s="6" t="s">
         <v>135</v>
@@ -9645,9 +9681,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="345" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A345" s="6" t="s">
-        <v>559</v>
+        <v>126</v>
       </c>
       <c r="B345" s="6" t="s">
         <v>135</v>
@@ -9665,43 +9701,123 @@
         <v>150</v>
       </c>
     </row>
-    <row r="346" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A346" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B346" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C346" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D346" t="s">
+        <v>134</v>
+      </c>
+      <c r="E346" t="s">
+        <v>147</v>
+      </c>
+      <c r="H346" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A347" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B347" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C347" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D347" t="s">
+        <v>134</v>
+      </c>
+      <c r="E347" t="s">
+        <v>147</v>
+      </c>
+      <c r="H347" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A348" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B348" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C348" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D348" t="s">
+        <v>134</v>
+      </c>
+      <c r="E348" t="s">
+        <v>147</v>
+      </c>
+      <c r="H348" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="349" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A349" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="B349" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C349" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D349" t="s">
+        <v>134</v>
+      </c>
+      <c r="E349" t="s">
+        <v>147</v>
+      </c>
+      <c r="H349" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="350" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A350" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B346" s="6" t="s">
+      <c r="B350" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C346" s="6" t="s">
+      <c r="C350" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="D346" t="s">
-        <v>134</v>
-      </c>
-      <c r="E346" t="s">
-        <v>147</v>
-      </c>
-      <c r="H346" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="347" spans="1:8" ht="345" x14ac:dyDescent="0.25">
-      <c r="A347" s="1" t="s">
+      <c r="D350" t="s">
+        <v>134</v>
+      </c>
+      <c r="E350" t="s">
+        <v>147</v>
+      </c>
+      <c r="H350" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="351" spans="1:8" ht="345" x14ac:dyDescent="0.25">
+      <c r="A351" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B347" s="6" t="s">
+      <c r="B351" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C347" s="11" t="s">
-        <v>560</v>
-      </c>
-      <c r="D347" t="s">
-        <v>134</v>
-      </c>
-      <c r="E347" t="s">
-        <v>147</v>
-      </c>
-      <c r="H347" t="s">
+      <c r="C351" s="11" t="s">
+        <v>558</v>
+      </c>
+      <c r="D351" t="s">
+        <v>134</v>
+      </c>
+      <c r="E351" t="s">
+        <v>147</v>
+      </c>
+      <c r="H351" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Singapore code updated with feedbacks
</commit_message>
<xml_diff>
--- a/Config/Singapore_Financial_Config.xlsx
+++ b/Config/Singapore_Financial_Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRADSOL123\PycharmProjects\MNS-Singapore\MNS-Singapore\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B68F458-B19F-47CF-9F66-6075D5088560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC18E8C9-99B1-4089-92B5-70103F91D201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$320</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$321</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2263" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2317" uniqueCount="629">
   <si>
     <t>Field_Name</t>
   </si>
@@ -1665,9 +1665,6 @@
     <t>Net Finance cost</t>
   </si>
   <si>
-    <t>finance_cost+finance_expenses+finance_costs+financial_costs+net_finance_cost</t>
-  </si>
-  <si>
     <t>Income tax</t>
   </si>
   <si>
@@ -1704,9 +1701,6 @@
     <t>minority_interest_and_profit_from_associates_and_joint_ventures</t>
   </si>
   <si>
-    <t xml:space="preserve">net_revenue +other_income+Revenue_from_Service+Other_Operating_Revenue+ Subsidy_Income+ Financial_Income+ Gains_Losses_Allocated_Subsidiaries_Associates_Joint_Ventures+ Income_Loss_from_Discontinued_Operations+ Group_Contribution_Received+ Non_Operating_Income- total_cost_of_materials_consumed - Power_Fuel-total_purchases_of_stock_in_trade - total_changes_in_inventories_or_finished_goods - total_employee_benefit_expense - total_other_expenses - depreciation- selling_expenses - administration_costs - Advertising_expense- Services- Auditors_Fee- Management_Expenses- Legal_Professional_Charges - Other_General_Expense- Repair_of_Machinery- depreciation- Personal_costs - Group_Contribution_Paid- Suppliers_And_External_Services- Impairment_Of_Investments_Not_Depreciable_Amortizable- interest - Other_Financial_Expenses + exceptional_items_before_tax  - income_tax - Current_Tax-Deferred_Tax -Advance_Tax-Other_Tax_Expenses+ profit_for_period_from_continuing_operations + profit_from_discontinuing_operation_after_tax - profit_after_tax </t>
-  </si>
-  <si>
     <t>Intangible_assets</t>
   </si>
   <si>
@@ -1815,9 +1809,6 @@
     <t>Share_of_results_of_equity_accounted_investees_net_of_tax</t>
   </si>
   <si>
-    <t>Other_income+other_income_gains_and_losses+other_gains_net+other_income_and_gains+Other_income_net+Share_of_results_of_equity_accounted_investees_net_of_tax</t>
-  </si>
-  <si>
     <t>financial_income</t>
   </si>
   <si>
@@ -1827,9 +1818,6 @@
     <t>Interest_income</t>
   </si>
   <si>
-    <t>Finance income+Interest_income</t>
-  </si>
-  <si>
     <t>Selling_expenses</t>
   </si>
   <si>
@@ -1861,6 +1849,72 @@
   </si>
   <si>
     <t>right_of_use+right_of_use_assets+Other_receivables+other_non_financial_assets+other_non_current_assets+others_noncurrent+other_noncurrent+Subsidiary_companies+Deposits+Derivatives</t>
+  </si>
+  <si>
+    <t>Other gains</t>
+  </si>
+  <si>
+    <t>Other_gains</t>
+  </si>
+  <si>
+    <t>Other_income+other_income_gains_and_losses+other_gains_net+other_income_and_gains+Other_income_net+Share_of_results_of_equity_accounted_investees_net_of_tax+Other_gains</t>
+  </si>
+  <si>
+    <t>financial_income+Interest_income</t>
+  </si>
+  <si>
+    <t>finance_expense</t>
+  </si>
+  <si>
+    <t>Finance expense</t>
+  </si>
+  <si>
+    <t>finance_cost+finance_expenses+finance_costs+financial_costs+net_finance_cost+finance_expense</t>
+  </si>
+  <si>
+    <t>profit_for_the_period</t>
+  </si>
+  <si>
+    <t>Profit for the period</t>
+  </si>
+  <si>
+    <t>profit_for_the_year</t>
+  </si>
+  <si>
+    <t>Profit for the year</t>
+  </si>
+  <si>
+    <t>profit_for_the_year_representing_total_comprehensive_income_for_the_year</t>
+  </si>
+  <si>
+    <t>Profit For The Year, Representing Total Comprehensive Income For The Year</t>
+  </si>
+  <si>
+    <t>profit_for_the_year_representing_total_comprehensive_income</t>
+  </si>
+  <si>
+    <t>Profit for the year, representing total comprehensive income for the year</t>
+  </si>
+  <si>
+    <t>loss_from_ordinary_activities_after_income_tax_and_total_comprehensive_loss_for_the_year</t>
+  </si>
+  <si>
+    <t>(Loss) from ordinary activities after income tax and total comprehensive (loss) for the year</t>
+  </si>
+  <si>
+    <t>net_profit_representing_total_comprehensive_income_for_the_year</t>
+  </si>
+  <si>
+    <t>Net profit, representing total comprehensive income for the year</t>
+  </si>
+  <si>
+    <t>profit_loss_for_the_year_representing_total_comprehensive_income_for_the_year</t>
+  </si>
+  <si>
+    <t>Profit/(Loss) for the year, representing total comprehensive income for the year</t>
+  </si>
+  <si>
+    <t>profit_after_tax-profit_for_the_period-profit_for_the_year-profit_for_the_year_representing_total_comprehensive_income_for_the_year-profit_for_the_year_representing_total_comprehensive_income-loss_from_ordinary_activities_after_income_tax_and_total_comprehensive_loss_for_the_year-net_profit_representing_total_comprehensive_income_for_the_year-profit_loss_for_the_year_representing_total_comprehensive_income_for_the_year</t>
   </si>
 </sst>
 </file>
@@ -2306,10 +2360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H352"/>
+  <dimension ref="A1:H361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
+      <selection activeCell="F356" sqref="F356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2685,7 +2739,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>135</v>
@@ -2760,7 +2814,7 @@
         <v>136</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D23" t="s">
         <v>134</v>
@@ -2846,13 +2900,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D27" t="s">
         <v>134</v>
@@ -2869,13 +2923,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D28" t="s">
         <v>134</v>
@@ -2898,7 +2952,7 @@
         <v>136</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D29" t="s">
         <v>134</v>
@@ -3536,13 +3590,13 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D57" t="s">
         <v>134</v>
@@ -3559,13 +3613,13 @@
     </row>
     <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D58" t="s">
         <v>134</v>
@@ -3588,7 +3642,7 @@
         <v>136</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="D59" t="s">
         <v>134</v>
@@ -3651,7 +3705,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>135</v>
@@ -3812,13 +3866,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D69" t="s">
         <v>134</v>
@@ -3841,7 +3895,7 @@
         <v>136</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="D70" t="s">
         <v>134</v>
@@ -4226,13 +4280,13 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="D87" t="s">
         <v>134</v>
@@ -4364,13 +4418,13 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C93" s="6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D93" t="s">
         <v>134</v>
@@ -4393,7 +4447,7 @@
         <v>136</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="D94" t="s">
         <v>134</v>
@@ -5123,13 +5177,13 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D126" t="s">
         <v>134</v>
@@ -5152,7 +5206,7 @@
         <v>136</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D127" t="s">
         <v>134</v>
@@ -5294,13 +5348,13 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D135" t="s">
         <v>134</v>
@@ -5317,13 +5371,13 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B136" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D136" t="s">
         <v>134</v>
@@ -5346,7 +5400,7 @@
         <v>136</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="D137" t="s">
         <v>134</v>
@@ -5616,13 +5670,13 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B149" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D149" t="s">
         <v>134</v>
@@ -5645,7 +5699,7 @@
         <v>136</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D150" t="s">
         <v>134</v>
@@ -5915,13 +5969,13 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="6" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B162" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D162" t="s">
         <v>134</v>
@@ -5944,7 +5998,7 @@
         <v>136</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D163" t="s">
         <v>134</v>
@@ -6122,13 +6176,13 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B171" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D171" t="s">
         <v>134</v>
@@ -6151,7 +6205,7 @@
         <v>136</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D172" t="s">
         <v>134</v>
@@ -6628,13 +6682,13 @@
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="6" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B193" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C193" s="6" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D193" t="s">
         <v>134</v>
@@ -6657,7 +6711,7 @@
         <v>136</v>
       </c>
       <c r="C194" s="6" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D194" t="s">
         <v>134</v>
@@ -6904,13 +6958,13 @@
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="6" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B205" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C205" s="6" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="D205" t="s">
         <v>134</v>
@@ -6933,7 +6987,7 @@
         <v>136</v>
       </c>
       <c r="C206" s="6" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D206" t="s">
         <v>134</v>
@@ -7249,13 +7303,13 @@
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="6" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B220" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C220" s="6" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D220" t="s">
         <v>134</v>
@@ -7278,7 +7332,7 @@
         <v>136</v>
       </c>
       <c r="C221" s="6" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D221" t="s">
         <v>134</v>
@@ -8155,7 +8209,7 @@
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268" s="6" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B268" s="6" t="s">
         <v>135</v>
@@ -8235,13 +8289,13 @@
     </row>
     <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272" s="6" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B272" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C272" s="6" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D272" t="s">
         <v>134</v>
@@ -8255,13 +8309,13 @@
     </row>
     <row r="273" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A273" s="6" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B273" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C273" s="6" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="D273" t="s">
         <v>134</v>
@@ -8273,35 +8327,35 @@
         <v>150</v>
       </c>
     </row>
-    <row r="274" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B274" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C274" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="D274" t="s">
+        <v>134</v>
+      </c>
+      <c r="E274" t="s">
+        <v>147</v>
+      </c>
+      <c r="H274" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A275" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B274" s="6" t="s">
+      <c r="B275" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C274" s="6" t="s">
-        <v>595</v>
-      </c>
-      <c r="D274" t="s">
-        <v>134</v>
-      </c>
-      <c r="E274" t="s">
-        <v>147</v>
-      </c>
-      <c r="H274" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A275" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B275" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C275" s="13" t="s">
-        <v>29</v>
+      <c r="C275" s="6" t="s">
+        <v>609</v>
       </c>
       <c r="D275" t="s">
         <v>134</v>
@@ -8315,13 +8369,13 @@
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B276" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C276" s="13" t="s">
-        <v>497</v>
+        <v>29</v>
       </c>
       <c r="D276" t="s">
         <v>134</v>
@@ -8335,33 +8389,33 @@
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B277" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C277" s="13" t="s">
+        <v>497</v>
+      </c>
+      <c r="D277" t="s">
+        <v>134</v>
+      </c>
+      <c r="E277" t="s">
+        <v>147</v>
+      </c>
+      <c r="H277" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A278" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B277" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C277" s="13" t="s">
+      <c r="B278" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C278" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="D277" t="s">
-        <v>134</v>
-      </c>
-      <c r="E277" t="s">
-        <v>147</v>
-      </c>
-      <c r="H277" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A278" s="14" t="s">
-        <v>596</v>
-      </c>
-      <c r="B278" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C278" s="15" t="s">
-        <v>498</v>
       </c>
       <c r="D278" t="s">
         <v>134</v>
@@ -8375,13 +8429,13 @@
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" s="14" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="B279" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C279" s="15" t="s">
-        <v>597</v>
+        <v>498</v>
       </c>
       <c r="D279" t="s">
         <v>134</v>
@@ -8394,34 +8448,34 @@
       </c>
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A280" s="6" t="s">
+      <c r="A280" s="14" t="s">
+        <v>595</v>
+      </c>
+      <c r="B280" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C280" s="15" t="s">
+        <v>594</v>
+      </c>
+      <c r="D280" t="s">
+        <v>134</v>
+      </c>
+      <c r="E280" t="s">
+        <v>147</v>
+      </c>
+      <c r="H280" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A281" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B280" s="6" t="s">
+      <c r="B281" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C280" s="6" t="s">
-        <v>599</v>
-      </c>
-      <c r="D280" t="s">
-        <v>134</v>
-      </c>
-      <c r="E280" t="s">
-        <v>147</v>
-      </c>
-      <c r="H280" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="281" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A281" s="6" t="s">
-        <v>499</v>
-      </c>
-      <c r="B281" s="6" t="s">
-        <v>135</v>
-      </c>
       <c r="C281" s="6" t="s">
-        <v>500</v>
+        <v>610</v>
       </c>
       <c r="D281" t="s">
         <v>134</v>
@@ -8435,13 +8489,13 @@
     </row>
     <row r="282" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A282" s="6" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B282" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C282" s="6" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D282" t="s">
         <v>134</v>
@@ -8455,13 +8509,13 @@
     </row>
     <row r="283" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A283" s="6" t="s">
-        <v>100</v>
+        <v>501</v>
       </c>
       <c r="B283" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C283" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D283" t="s">
         <v>134</v>
@@ -8475,27 +8529,27 @@
     </row>
     <row r="284" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A284" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B284" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C284" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="D284" t="s">
+        <v>134</v>
+      </c>
+      <c r="E284" t="s">
+        <v>147</v>
+      </c>
+      <c r="H284" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A285" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="B284" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C284" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D284" t="s">
-        <v>134</v>
-      </c>
-      <c r="E284" t="s">
-        <v>147</v>
-      </c>
-      <c r="H284" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A285" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="B285" s="6" t="s">
         <v>135</v>
@@ -8513,15 +8567,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="286" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286" s="6" t="s">
-        <v>504</v>
+        <v>102</v>
       </c>
       <c r="B286" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C286" s="6" t="s">
-        <v>505</v>
+        <v>29</v>
       </c>
       <c r="D286" t="s">
         <v>134</v>
@@ -8535,53 +8589,53 @@
     </row>
     <row r="287" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A287" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="B287" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C287" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="D287" t="s">
+        <v>134</v>
+      </c>
+      <c r="E287" t="s">
+        <v>147</v>
+      </c>
+      <c r="H287" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="288" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A288" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="B287" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C287" s="6" t="s">
+      <c r="B288" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C288" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="D287" t="s">
-        <v>134</v>
-      </c>
-      <c r="E287" t="s">
-        <v>147</v>
-      </c>
-      <c r="H287" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="288" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A288" s="6" t="s">
+      <c r="D288" t="s">
+        <v>134</v>
+      </c>
+      <c r="E288" t="s">
+        <v>147</v>
+      </c>
+      <c r="H288" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A289" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B288" s="6" t="s">
+      <c r="B289" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C288" s="6" t="s">
+      <c r="C289" s="6" t="s">
         <v>508</v>
-      </c>
-      <c r="D288" t="s">
-        <v>134</v>
-      </c>
-      <c r="E288" t="s">
-        <v>147</v>
-      </c>
-      <c r="H288" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A289" s="6" t="s">
-        <v>600</v>
-      </c>
-      <c r="B289" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C289" s="6" t="s">
-        <v>509</v>
       </c>
       <c r="D289" t="s">
         <v>134</v>
@@ -8595,53 +8649,53 @@
     </row>
     <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="B290" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C290" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="D290" t="s">
+        <v>134</v>
+      </c>
+      <c r="E290" t="s">
+        <v>147</v>
+      </c>
+      <c r="H290" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A291" s="6" t="s">
         <v>510</v>
       </c>
-      <c r="B290" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C290" s="6" t="s">
+      <c r="B291" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C291" s="6" t="s">
         <v>511</v>
       </c>
-      <c r="D290" t="s">
-        <v>134</v>
-      </c>
-      <c r="E290" t="s">
-        <v>147</v>
-      </c>
-      <c r="H290" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="291" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A291" s="6" t="s">
+      <c r="D291" t="s">
+        <v>134</v>
+      </c>
+      <c r="E291" t="s">
+        <v>147</v>
+      </c>
+      <c r="H291" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="292" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A292" s="6" t="s">
         <v>512</v>
       </c>
-      <c r="B291" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C291" s="6" t="s">
+      <c r="B292" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C292" s="6" t="s">
         <v>513</v>
-      </c>
-      <c r="D291" t="s">
-        <v>134</v>
-      </c>
-      <c r="E291" t="s">
-        <v>147</v>
-      </c>
-      <c r="H291" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A292" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="B292" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C292" s="6" t="s">
-        <v>271</v>
       </c>
       <c r="D292" t="s">
         <v>134</v>
@@ -8655,13 +8709,13 @@
     </row>
     <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293" s="6" t="s">
-        <v>514</v>
+        <v>270</v>
       </c>
       <c r="B293" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C293" s="6" t="s">
-        <v>515</v>
+        <v>271</v>
       </c>
       <c r="D293" t="s">
         <v>134</v>
@@ -8675,13 +8729,13 @@
     </row>
     <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294" s="6" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B294" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C294" s="6" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D294" t="s">
         <v>134</v>
@@ -8695,33 +8749,33 @@
     </row>
     <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295" s="6" t="s">
+        <v>516</v>
+      </c>
+      <c r="B295" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C295" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="D295" t="s">
+        <v>134</v>
+      </c>
+      <c r="E295" t="s">
+        <v>147</v>
+      </c>
+      <c r="H295" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A296" s="6" t="s">
         <v>518</v>
       </c>
-      <c r="B295" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C295" s="6" t="s">
+      <c r="B296" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C296" s="6" t="s">
         <v>519</v>
-      </c>
-      <c r="D295" t="s">
-        <v>134</v>
-      </c>
-      <c r="E295" t="s">
-        <v>147</v>
-      </c>
-      <c r="H295" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="296" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A296" s="6" t="s">
-        <v>520</v>
-      </c>
-      <c r="B296" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C296" s="6" t="s">
-        <v>521</v>
       </c>
       <c r="D296" t="s">
         <v>134</v>
@@ -8735,13 +8789,13 @@
     </row>
     <row r="297" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A297" s="6" t="s">
-        <v>602</v>
+        <v>520</v>
       </c>
       <c r="B297" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C297" s="6" t="s">
-        <v>601</v>
+        <v>521</v>
       </c>
       <c r="D297" t="s">
         <v>134</v>
@@ -8753,35 +8807,35 @@
         <v>150</v>
       </c>
     </row>
-    <row r="298" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A298" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="B298" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C298" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="D298" t="s">
+        <v>134</v>
+      </c>
+      <c r="E298" t="s">
+        <v>147</v>
+      </c>
+      <c r="H298" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="299" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A299" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B298" s="6" t="s">
+      <c r="B299" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C298" s="6" t="s">
-        <v>603</v>
-      </c>
-      <c r="D298" t="s">
-        <v>134</v>
-      </c>
-      <c r="E298" t="s">
-        <v>147</v>
-      </c>
-      <c r="H298" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A299" s="6" t="s">
-        <v>522</v>
-      </c>
-      <c r="B299" s="6" t="s">
-        <v>135</v>
-      </c>
       <c r="C299" s="6" t="s">
-        <v>523</v>
+        <v>599</v>
       </c>
       <c r="D299" t="s">
         <v>134</v>
@@ -8795,13 +8849,13 @@
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300" s="6" t="s">
-        <v>272</v>
+        <v>522</v>
       </c>
       <c r="B300" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C300" s="6" t="s">
-        <v>273</v>
+        <v>523</v>
       </c>
       <c r="D300" t="s">
         <v>134</v>
@@ -8815,33 +8869,33 @@
     </row>
     <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A301" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="B301" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C301" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="D301" t="s">
+        <v>134</v>
+      </c>
+      <c r="E301" t="s">
+        <v>147</v>
+      </c>
+      <c r="H301" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A302" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="B301" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C301" s="6" t="s">
+      <c r="B302" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C302" s="6" t="s">
         <v>525</v>
-      </c>
-      <c r="D301" t="s">
-        <v>134</v>
-      </c>
-      <c r="E301" t="s">
-        <v>147</v>
-      </c>
-      <c r="H301" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="302" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A302" s="6" t="s">
-        <v>526</v>
-      </c>
-      <c r="B302" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C302" s="6" t="s">
-        <v>527</v>
       </c>
       <c r="D302" t="s">
         <v>134</v>
@@ -8855,33 +8909,33 @@
     </row>
     <row r="303" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A303" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="B303" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C303" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="D303" t="s">
+        <v>134</v>
+      </c>
+      <c r="E303" t="s">
+        <v>147</v>
+      </c>
+      <c r="H303" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="304" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A304" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B303" s="6" t="s">
+      <c r="B304" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C303" s="6" t="s">
+      <c r="C304" s="6" t="s">
         <v>528</v>
-      </c>
-      <c r="D303" t="s">
-        <v>134</v>
-      </c>
-      <c r="E303" t="s">
-        <v>147</v>
-      </c>
-      <c r="H303" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A304" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="B304" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C304" s="6" t="s">
-        <v>275</v>
       </c>
       <c r="D304" t="s">
         <v>134</v>
@@ -8895,13 +8949,13 @@
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B305" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C305" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D305" t="s">
         <v>134</v>
@@ -8915,13 +8969,13 @@
     </row>
     <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306" s="6" t="s">
-        <v>106</v>
+        <v>276</v>
       </c>
       <c r="B306" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C306" s="6" t="s">
-        <v>529</v>
+        <v>277</v>
       </c>
       <c r="D306" t="s">
         <v>134</v>
@@ -8935,13 +8989,13 @@
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B307" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C307" s="6" t="s">
-        <v>29</v>
+        <v>529</v>
       </c>
       <c r="D307" t="s">
         <v>134</v>
@@ -8955,7 +9009,7 @@
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B308" s="6" t="s">
         <v>135</v>
@@ -8975,7 +9029,7 @@
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B309" s="6" t="s">
         <v>135</v>
@@ -8995,7 +9049,7 @@
     </row>
     <row r="310" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A310" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B310" s="6" t="s">
         <v>135</v>
@@ -9015,7 +9069,7 @@
     </row>
     <row r="311" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A311" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B311" s="6" t="s">
         <v>135</v>
@@ -9035,7 +9089,7 @@
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A312" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B312" s="6" t="s">
         <v>135</v>
@@ -9053,55 +9107,55 @@
         <v>150</v>
       </c>
     </row>
-    <row r="313" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A313" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B313" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C313" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D313" t="s">
+        <v>134</v>
+      </c>
+      <c r="E313" t="s">
+        <v>147</v>
+      </c>
+      <c r="H313" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="314" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A314" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="B313" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C313" s="6" t="s">
+      <c r="B314" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C314" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="D313" t="s">
-        <v>134</v>
-      </c>
-      <c r="E313" t="s">
-        <v>147</v>
-      </c>
-      <c r="H313" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A314" s="6" t="s">
+      <c r="D314" t="s">
+        <v>134</v>
+      </c>
+      <c r="E314" t="s">
+        <v>147</v>
+      </c>
+      <c r="H314" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A315" s="6" t="s">
         <v>530</v>
       </c>
-      <c r="B314" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C314" s="6" t="s">
+      <c r="B315" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C315" s="6" t="s">
         <v>531</v>
-      </c>
-      <c r="D314" t="s">
-        <v>134</v>
-      </c>
-      <c r="E314" t="s">
-        <v>147</v>
-      </c>
-      <c r="H314" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="315" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A315" s="6" t="s">
-        <v>532</v>
-      </c>
-      <c r="B315" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C315" s="6" t="s">
-        <v>533</v>
       </c>
       <c r="D315" t="s">
         <v>134</v>
@@ -9115,93 +9169,93 @@
     </row>
     <row r="316" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A316" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="B316" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C316" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="D316" t="s">
+        <v>134</v>
+      </c>
+      <c r="E316" t="s">
+        <v>147</v>
+      </c>
+      <c r="H316" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="317" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A317" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="B316" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C316" s="6" t="s">
+      <c r="B317" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C317" s="6" t="s">
         <v>535</v>
       </c>
-      <c r="D316" t="s">
-        <v>134</v>
-      </c>
-      <c r="E316" t="s">
-        <v>147</v>
-      </c>
-      <c r="H316" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A317" s="6" t="s">
+      <c r="D317" t="s">
+        <v>134</v>
+      </c>
+      <c r="E317" t="s">
+        <v>147</v>
+      </c>
+      <c r="H317" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A318" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B317" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C317" s="6" t="s">
+      <c r="B318" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C318" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="D317" t="s">
-        <v>134</v>
-      </c>
-      <c r="E317" t="s">
-        <v>147</v>
-      </c>
-      <c r="H317" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="318" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A318" s="6" t="s">
+      <c r="D318" t="s">
+        <v>134</v>
+      </c>
+      <c r="E318" t="s">
+        <v>147</v>
+      </c>
+      <c r="H318" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="319" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A319" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="B318" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C318" s="6" t="s">
+      <c r="B319" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C319" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="D318" t="s">
-        <v>134</v>
-      </c>
-      <c r="E318" t="s">
-        <v>147</v>
-      </c>
-      <c r="H318" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="319" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A319" s="6" t="s">
+      <c r="D319" t="s">
+        <v>134</v>
+      </c>
+      <c r="E319" t="s">
+        <v>147</v>
+      </c>
+      <c r="H319" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="320" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A320" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B319" s="6" t="s">
+      <c r="B320" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C319" s="6" t="s">
+      <c r="C320" s="6" t="s">
         <v>537</v>
-      </c>
-      <c r="D319" t="s">
-        <v>134</v>
-      </c>
-      <c r="E319" t="s">
-        <v>147</v>
-      </c>
-      <c r="H319" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A320" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B320" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C320" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="D320" t="s">
         <v>134</v>
@@ -9215,7 +9269,7 @@
     </row>
     <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B321" s="6" t="s">
         <v>135</v>
@@ -9235,7 +9289,7 @@
     </row>
     <row r="322" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A322" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B322" s="6" t="s">
         <v>135</v>
@@ -9253,55 +9307,55 @@
         <v>150</v>
       </c>
     </row>
-    <row r="323" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A323" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B323" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C323" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D323" t="s">
+        <v>134</v>
+      </c>
+      <c r="E323" t="s">
+        <v>147</v>
+      </c>
+      <c r="H323" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="324" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A324" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B323" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C323" s="6" t="s">
+      <c r="B324" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C324" s="6" t="s">
         <v>538</v>
       </c>
-      <c r="D323" t="s">
-        <v>134</v>
-      </c>
-      <c r="E323" t="s">
-        <v>147</v>
-      </c>
-      <c r="H323" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="324" spans="1:8" ht="195" x14ac:dyDescent="0.25">
-      <c r="A324" s="6" t="s">
+      <c r="D324" t="s">
+        <v>134</v>
+      </c>
+      <c r="E324" t="s">
+        <v>147</v>
+      </c>
+      <c r="H324" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="325" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="A325" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B324" s="6" t="s">
+      <c r="B325" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C324" s="6" t="s">
+      <c r="C325" s="6" t="s">
         <v>282</v>
-      </c>
-      <c r="D324" t="s">
-        <v>134</v>
-      </c>
-      <c r="E324" t="s">
-        <v>147</v>
-      </c>
-      <c r="H324" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A325" s="6" t="s">
-        <v>539</v>
-      </c>
-      <c r="B325" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C325" s="6" t="s">
-        <v>540</v>
       </c>
       <c r="D325" t="s">
         <v>134</v>
@@ -9315,13 +9369,13 @@
     </row>
     <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326" s="6" t="s">
-        <v>284</v>
+        <v>539</v>
       </c>
       <c r="B326" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C326" s="6" t="s">
-        <v>149</v>
+        <v>540</v>
       </c>
       <c r="D326" t="s">
         <v>134</v>
@@ -9335,13 +9389,13 @@
     </row>
     <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327" s="6" t="s">
-        <v>148</v>
+        <v>284</v>
       </c>
       <c r="B327" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C327" s="6" t="s">
-        <v>283</v>
+        <v>149</v>
       </c>
       <c r="D327" t="s">
         <v>134</v>
@@ -9355,13 +9409,13 @@
     </row>
     <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328" s="6" t="s">
-        <v>541</v>
+        <v>148</v>
       </c>
       <c r="B328" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C328" s="6" t="s">
-        <v>542</v>
+        <v>283</v>
       </c>
       <c r="D328" t="s">
         <v>134</v>
@@ -9375,33 +9429,33 @@
     </row>
     <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329" s="6" t="s">
+        <v>541</v>
+      </c>
+      <c r="B329" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C329" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="D329" t="s">
+        <v>134</v>
+      </c>
+      <c r="E329" t="s">
+        <v>147</v>
+      </c>
+      <c r="H329" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A330" s="6" t="s">
         <v>543</v>
       </c>
-      <c r="B329" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C329" s="6" t="s">
+      <c r="B330" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C330" s="6" t="s">
         <v>544</v>
-      </c>
-      <c r="D329" t="s">
-        <v>134</v>
-      </c>
-      <c r="E329" t="s">
-        <v>147</v>
-      </c>
-      <c r="H329" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="330" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A330" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B330" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C330" s="6" t="s">
-        <v>545</v>
       </c>
       <c r="D330" t="s">
         <v>134</v>
@@ -9415,13 +9469,13 @@
     </row>
     <row r="331" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A331" s="6" t="s">
-        <v>120</v>
+        <v>611</v>
       </c>
       <c r="B331" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C331" s="6" t="s">
-        <v>29</v>
+        <v>612</v>
       </c>
       <c r="D331" t="s">
         <v>134</v>
@@ -9435,13 +9489,13 @@
     </row>
     <row r="332" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A332" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B332" s="6" t="s">
         <v>136</v>
       </c>
       <c r="C332" s="6" t="s">
-        <v>122</v>
+        <v>613</v>
       </c>
       <c r="D332" t="s">
         <v>134</v>
@@ -9455,7 +9509,7 @@
     </row>
     <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B333" s="6" t="s">
         <v>135</v>
@@ -9475,13 +9529,13 @@
     </row>
     <row r="334" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A334" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B334" s="6" t="s">
         <v>136</v>
       </c>
       <c r="C334" s="6" t="s">
-        <v>285</v>
+        <v>122</v>
       </c>
       <c r="D334" t="s">
         <v>134</v>
@@ -9495,13 +9549,13 @@
     </row>
     <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335" s="6" t="s">
-        <v>286</v>
+        <v>123</v>
       </c>
       <c r="B335" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C335" s="6" t="s">
-        <v>287</v>
+        <v>29</v>
       </c>
       <c r="D335" t="s">
         <v>134</v>
@@ -9513,15 +9567,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A336" s="6" t="s">
-        <v>288</v>
+        <v>124</v>
       </c>
       <c r="B336" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C336" s="6" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D336" t="s">
         <v>134</v>
@@ -9535,13 +9589,13 @@
     </row>
     <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337" s="6" t="s">
-        <v>604</v>
+        <v>286</v>
       </c>
       <c r="B337" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C337" s="6" t="s">
-        <v>546</v>
+        <v>287</v>
       </c>
       <c r="D337" t="s">
         <v>134</v>
@@ -9555,13 +9609,13 @@
     </row>
     <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338" s="6" t="s">
-        <v>547</v>
+        <v>288</v>
       </c>
       <c r="B338" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C338" s="6" t="s">
-        <v>548</v>
+        <v>289</v>
       </c>
       <c r="D338" t="s">
         <v>134</v>
@@ -9575,13 +9629,13 @@
     </row>
     <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339" s="6" t="s">
-        <v>549</v>
+        <v>600</v>
       </c>
       <c r="B339" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C339" s="6" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="D339" t="s">
         <v>134</v>
@@ -9595,13 +9649,13 @@
     </row>
     <row r="340" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A340" s="6" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="B340" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C340" s="6" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="D340" t="s">
         <v>134</v>
@@ -9615,13 +9669,13 @@
     </row>
     <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341" s="6" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="B341" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C341" s="6" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="D341" t="s">
         <v>134</v>
@@ -9635,87 +9689,87 @@
     </row>
     <row r="342" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A342" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="B342" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C342" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="D342" t="s">
+        <v>134</v>
+      </c>
+      <c r="E342" t="s">
+        <v>147</v>
+      </c>
+      <c r="H342" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A343" s="6" t="s">
+        <v>552</v>
+      </c>
+      <c r="B343" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C343" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="D343" t="s">
+        <v>134</v>
+      </c>
+      <c r="E343" t="s">
+        <v>147</v>
+      </c>
+      <c r="H343" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A344" s="6" t="s">
+        <v>554</v>
+      </c>
+      <c r="B344" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C344" s="6" t="s">
         <v>555</v>
       </c>
-      <c r="B342" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C342" s="6" t="s">
-        <v>556</v>
-      </c>
-      <c r="D342" t="s">
-        <v>134</v>
-      </c>
-      <c r="E342" t="s">
-        <v>147</v>
-      </c>
-      <c r="H342" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="343" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A343" s="6" t="s">
+      <c r="D344" t="s">
+        <v>134</v>
+      </c>
+      <c r="E344" t="s">
+        <v>147</v>
+      </c>
+      <c r="H344" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="345" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A345" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B343" s="6" t="s">
+      <c r="B345" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C343" s="6" t="s">
-        <v>605</v>
-      </c>
-      <c r="D343" t="s">
-        <v>134</v>
-      </c>
-      <c r="E343" t="s">
-        <v>147</v>
-      </c>
-      <c r="H343" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="344" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A344" s="6" t="s">
+      <c r="C345" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="D345" t="s">
+        <v>134</v>
+      </c>
+      <c r="E345" t="s">
+        <v>147</v>
+      </c>
+      <c r="H345" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="346" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A346" s="6" t="s">
         <v>130</v>
-      </c>
-      <c r="B344" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C344" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D344" t="s">
-        <v>134</v>
-      </c>
-      <c r="E344" t="s">
-        <v>147</v>
-      </c>
-      <c r="H344" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="345" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A345" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B345" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C345" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D345" t="s">
-        <v>134</v>
-      </c>
-      <c r="E345" t="s">
-        <v>147</v>
-      </c>
-      <c r="H345" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A346" s="6" t="s">
-        <v>126</v>
       </c>
       <c r="B346" s="6" t="s">
         <v>135</v>
@@ -9733,9 +9787,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A347" s="6" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B347" s="6" t="s">
         <v>135</v>
@@ -9755,7 +9809,7 @@
     </row>
     <row r="348" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A348" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B348" s="6" t="s">
         <v>135</v>
@@ -9775,7 +9829,7 @@
     </row>
     <row r="349" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A349" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B349" s="6" t="s">
         <v>135</v>
@@ -9793,9 +9847,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="350" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A350" s="6" t="s">
-        <v>557</v>
+        <v>128</v>
       </c>
       <c r="B350" s="6" t="s">
         <v>135</v>
@@ -9813,43 +9867,223 @@
         <v>150</v>
       </c>
     </row>
-    <row r="351" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A351" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B351" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C351" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D351" t="s">
+        <v>134</v>
+      </c>
+      <c r="E351" t="s">
+        <v>147</v>
+      </c>
+      <c r="H351" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="352" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A352" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="B352" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C352" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D352" t="s">
+        <v>134</v>
+      </c>
+      <c r="E352" t="s">
+        <v>147</v>
+      </c>
+      <c r="H352" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="353" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A353" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B351" s="6" t="s">
+      <c r="B353" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C351" s="6" t="s">
+      <c r="C353" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="D351" t="s">
-        <v>134</v>
-      </c>
-      <c r="E351" t="s">
-        <v>147</v>
-      </c>
-      <c r="H351" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="352" spans="1:8" ht="345" x14ac:dyDescent="0.25">
-      <c r="A352" s="1" t="s">
+      <c r="D353" t="s">
+        <v>134</v>
+      </c>
+      <c r="E353" t="s">
+        <v>147</v>
+      </c>
+      <c r="H353" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A354" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="B354" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C354" s="6" t="s">
+        <v>615</v>
+      </c>
+      <c r="D354" t="s">
+        <v>134</v>
+      </c>
+      <c r="E354" t="s">
+        <v>147</v>
+      </c>
+      <c r="H354" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A355" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="B355" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C355" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="D355" t="s">
+        <v>134</v>
+      </c>
+      <c r="E355" t="s">
+        <v>147</v>
+      </c>
+      <c r="H355" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="356" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A356" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="B356" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C356" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="D356" t="s">
+        <v>134</v>
+      </c>
+      <c r="E356" t="s">
+        <v>147</v>
+      </c>
+      <c r="H356" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="357" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A357" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="B357" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C357" s="6" t="s">
+        <v>621</v>
+      </c>
+      <c r="D357" t="s">
+        <v>134</v>
+      </c>
+      <c r="E357" t="s">
+        <v>147</v>
+      </c>
+      <c r="H357" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="358" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A358" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="B358" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C358" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="D358" t="s">
+        <v>134</v>
+      </c>
+      <c r="E358" t="s">
+        <v>147</v>
+      </c>
+      <c r="H358" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="359" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A359" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="B359" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C359" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="D359" t="s">
+        <v>134</v>
+      </c>
+      <c r="E359" t="s">
+        <v>147</v>
+      </c>
+      <c r="H359" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="360" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A360" s="6" t="s">
+        <v>626</v>
+      </c>
+      <c r="B360" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C360" s="6" t="s">
+        <v>627</v>
+      </c>
+      <c r="D360" t="s">
+        <v>134</v>
+      </c>
+      <c r="E360" t="s">
+        <v>147</v>
+      </c>
+      <c r="H360" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="361" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A361" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B352" s="6" t="s">
+      <c r="B361" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C352" s="11" t="s">
-        <v>558</v>
-      </c>
-      <c r="D352" t="s">
-        <v>134</v>
-      </c>
-      <c r="E352" t="s">
-        <v>147</v>
-      </c>
-      <c r="H352" t="s">
+      <c r="C361" s="11" t="s">
+        <v>628</v>
+      </c>
+      <c r="D361" t="s">
+        <v>134</v>
+      </c>
+      <c r="E361" t="s">
+        <v>147</v>
+      </c>
+      <c r="H361" t="s">
         <v>150</v>
       </c>
     </row>

</xml_diff>